<commit_message>
Update xlsx (forgot 'note')
</commit_message>
<xml_diff>
--- a/app/config/tables/datesTest/forms/datesTest/datesTest.xlsx
+++ b/app/config/tables/datesTest/forms/datesTest/datesTest.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t xml:space="preserve">comments</t>
   </si>
@@ -199,10 +199,19 @@
     <t xml:space="preserve">data('test3') &gt; 100</t>
   </si>
   <si>
+    <t xml:space="preserve">Will exit section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will not exit section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end if</t>
+  </si>
+  <si>
     <t xml:space="preserve">exit section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end if</t>
   </si>
   <si>
     <t xml:space="preserve">test4</t>
@@ -979,10 +988,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1048,66 +1057,100 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>55</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>56</v>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
-        <v>58</v>
+      <c r="D8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>60</v>
+      <c r="B10" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="s">
-        <v>18</v>
+      <c r="B11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="0" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3" t="s">
+      <c r="F18" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"fix" do section at the end of the 'survey' section bug
</commit_message>
<xml_diff>
--- a/app/config/tables/datesTest/forms/datesTest/datesTest.xlsx
+++ b/app/config/tables/datesTest/forms/datesTest/datesTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,8 @@
     <sheet name="settings" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="model" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Sheet7" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="soi" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="smg" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="89">
   <si>
     <t xml:space="preserve">comments</t>
   </si>
@@ -91,12 +93,78 @@
     <t xml:space="preserve">Back in survey section</t>
   </si>
   <si>
+    <t xml:space="preserve">select_multiple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_sections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What other sections to go to?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(data('other_sections'), 'select one integer')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do section soi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(data('other_sections'), 'select multiple grid')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do section smg</t>
+  </si>
+  <si>
     <t xml:space="preserve">choice_list_name</t>
   </si>
   <si>
     <t xml:space="preserve">data_value</t>
   </si>
   <si>
+    <t xml:space="preserve">display.title.image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select one integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select multiple grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">earworm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">media/earworm.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stink_bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">media/stink_bug.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cutworm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">media/cutworm.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beetle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">media/corn_flea_beetle.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">query_name</t>
   </si>
   <si>
@@ -193,9 +261,6 @@
     <t xml:space="preserve">If you enter a number greater than 100, I will execute “exit section”. Otherwise, you will pass through two more screens in this section</t>
   </si>
   <si>
-    <t xml:space="preserve">if</t>
-  </si>
-  <si>
     <t xml:space="preserve">data('test3') &gt; 100</t>
   </si>
   <si>
@@ -208,9 +273,6 @@
     <t xml:space="preserve">Will not exit section</t>
   </si>
   <si>
-    <t xml:space="preserve">end if</t>
-  </si>
-  <si>
     <t xml:space="preserve">exit section</t>
   </si>
   <si>
@@ -224,6 +286,15 @@
   </si>
   <si>
     <t xml:space="preserve">This is the last screen in section Sheet7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one_integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_multiple_grid</t>
   </si>
 </sst>
 </file>
@@ -452,8 +523,8 @@
   </sheetPr>
   <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C3 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -590,13 +661,56 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="16" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="23.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -664,10 +778,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -680,25 +794,134 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="D1" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>2014</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -734,7 +957,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -753,37 +976,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -808,7 +1031,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="C3 E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -820,36 +1043,36 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -873,7 +1096,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="C3 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -886,10 +1109,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>6</v>
@@ -897,23 +1120,23 @@
     </row>
     <row r="2" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>20170729</v>
@@ -921,15 +1144,15 @@
     </row>
     <row r="5" customFormat="false" ht="16.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>10</v>
@@ -956,7 +1179,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C3 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -990,8 +1213,8 @@
   </sheetPr>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="1" sqref="C3 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1041,26 +1264,26 @@
         <v>15</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,12 +1291,12 @@
         <v>15</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,12 +1304,12 @@
         <v>15</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,20 +1319,20 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1122,10 +1345,10 @@
         <v>9</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,15 +1366,137 @@
         <v>12</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="C3 E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="C3 E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>